<commit_message>
Modified to add cases 6/28
</commit_message>
<xml_diff>
--- a/examples/Generator_expansion/data.xlsx
+++ b/examples/Generator_expansion/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camerin/Desktop/Sensitivity Analysis/cap expansion data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PAMSO.jl\examples\Generator_expansion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2208EEFF-C958-CC44-AB05-179082BF56D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DED75C-396A-49BD-B29D-23D43FF78838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="4" xr2:uid="{55ABDE78-1F70-46C0-8258-C13FCFD69A49}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{55ABDE78-1F70-46C0-8258-C13FCFD69A49}"/>
   </bookViews>
   <sheets>
     <sheet name="DIC" sheetId="1" r:id="rId1"/>
@@ -447,13 +447,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C23A72-8ADB-4B21-9418-BC968A403312}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,18 +464,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -496,12 +496,12 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -523,7 +523,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -534,7 +534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -545,7 +545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -556,7 +556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -567,7 +567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -591,9 +591,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -601,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -609,7 +609,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -617,7 +617,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -638,9 +638,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -669,7 +669,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -684,7 +684,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -699,7 +699,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -714,7 +714,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -728,7 +728,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -742,7 +742,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -756,7 +756,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -770,7 +770,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -785,7 +785,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -800,7 +800,7 @@
         <v>666.66666666666674</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -815,7 +815,7 @@
         <v>1666.6666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -839,13 +839,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FC0697-257E-45E2-AE93-E6D277F7F6D3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -856,7 +856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -867,7 +867,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -878,7 +878,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -889,7 +889,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -913,9 +913,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -926,7 +926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -937,7 +937,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -959,7 +959,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -970,7 +970,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>